<commit_message>
* added computed attributes
</commit_message>
<xml_diff>
--- a/TourPlanner_Checklist.xlsx
+++ b/TourPlanner_Checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainf\Desktop\FH Technikum Offline\TourPlanner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38AF57C3-3F8B-4EA8-9CF9-7B17D6538ED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{129C19AC-E328-434E-94F2-F5DBE3506DA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2240" yWindow="2240" windowWidth="19200" windowHeight="9970" xr2:uid="{88369686-F968-45CB-887F-E38F2E727DD7}"/>
+    <workbookView xWindow="1900" yWindow="1900" windowWidth="19200" windowHeight="9970" xr2:uid="{88369686-F968-45CB-887F-E38F2E727DD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="67">
   <si>
     <t>Checklist Tourplanner Exam 2</t>
   </si>
@@ -669,8 +669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D58600B0-3567-4A3D-A785-925E0537D06D}">
   <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -945,8 +945,8 @@
       <c r="C34" s="6">
         <v>2</v>
       </c>
-      <c r="D34" t="s">
-        <v>66</v>
+      <c r="D34">
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
@@ -956,8 +956,8 @@
       <c r="C35" s="6">
         <v>2</v>
       </c>
-      <c r="D35" t="s">
-        <v>66</v>
+      <c r="D35">
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
@@ -1333,6 +1333,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010075D40D9C3EDB8943872FF524C6B3FD0A" ma:contentTypeVersion="3" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="c8b69379abfde7286eda3659b10c0c3d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0dd4ebbd-e603-4963-8782-ab9329a1459d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="455ee242f80cd7a09b1a6ea5707d2ed2" ns2:_="">
     <xsd:import namespace="0dd4ebbd-e603-4963-8782-ab9329a1459d"/>
@@ -1470,22 +1485,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{981279ED-D6DF-4F74-A002-827C305FADC6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3CEAD3D1-BC7F-4367-835C-54F9567E9A4E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{536D9EC2-1905-4286-971A-18C563B29D4A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1501,21 +1518,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3CEAD3D1-BC7F-4367-835C-54F9567E9A4E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{981279ED-D6DF-4F74-A002-827C305FADC6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
* removed singleton pattern from repositories in favor of composition
</commit_message>
<xml_diff>
--- a/TourPlanner_Checklist.xlsx
+++ b/TourPlanner_Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainf\Desktop\FH Technikum Offline\TourPlanner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{129C19AC-E328-434E-94F2-F5DBE3506DA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBBE7F5F-8AF3-4819-B90B-C5FEC60DD188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1900" yWindow="1900" windowWidth="19200" windowHeight="9970" xr2:uid="{88369686-F968-45CB-887F-E38F2E727DD7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="67">
   <si>
     <t>Checklist Tourplanner Exam 2</t>
   </si>
@@ -669,8 +669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D58600B0-3567-4A3D-A785-925E0537D06D}">
   <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -967,8 +967,8 @@
       <c r="C36" s="6">
         <v>1</v>
       </c>
-      <c r="D36" t="s">
-        <v>66</v>
+      <c r="D36">
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
* refactored tourlog logic into separate VM, TODO: Fix cross viewmodel update
</commit_message>
<xml_diff>
--- a/TourPlanner_Checklist.xlsx
+++ b/TourPlanner_Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainf\Desktop\FH Technikum Offline\TourPlanner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBBE7F5F-8AF3-4819-B90B-C5FEC60DD188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F984F51-AB4D-4381-A63A-257A7AC554DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1900" yWindow="1900" windowWidth="19200" windowHeight="9970" xr2:uid="{88369686-F968-45CB-887F-E38F2E727DD7}"/>
   </bookViews>
@@ -669,8 +669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D58600B0-3567-4A3D-A785-925E0537D06D}">
   <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
* started with documentation
</commit_message>
<xml_diff>
--- a/TourPlanner_Checklist.xlsx
+++ b/TourPlanner_Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mainf\Desktop\FH Technikum Offline\TourPlanner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB7E0B1-6F43-47EE-9802-868D082E92BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A587851-9D05-487E-93FF-022C22E605D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="2640" windowWidth="29040" windowHeight="15720" xr2:uid="{88369686-F968-45CB-887F-E38F2E727DD7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="67">
   <si>
     <t>Checklist Tourplanner Exam 2</t>
   </si>
@@ -670,7 +670,7 @@
   <dimension ref="A1:D79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -908,7 +908,7 @@
         <v>2</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:4" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
@@ -1209,8 +1209,8 @@
       <c r="C67" s="6">
         <v>3</v>
       </c>
-      <c r="D67" t="s">
-        <v>66</v>
+      <c r="D67">
+        <v>3</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
@@ -1242,8 +1242,8 @@
       <c r="C70" s="6">
         <v>1</v>
       </c>
-      <c r="D70" t="s">
-        <v>66</v>
+      <c r="D70">
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
@@ -1253,8 +1253,8 @@
       <c r="C71" s="6">
         <v>1</v>
       </c>
-      <c r="D71" t="s">
-        <v>66</v>
+      <c r="D71">
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
@@ -1264,8 +1264,8 @@
       <c r="C72" s="6">
         <v>1</v>
       </c>
-      <c r="D72" t="s">
-        <v>66</v>
+      <c r="D72">
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
@@ -1275,8 +1275,8 @@
       <c r="C73" s="6">
         <v>1</v>
       </c>
-      <c r="D73" t="s">
-        <v>66</v>
+      <c r="D73">
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
@@ -1286,8 +1286,8 @@
       <c r="C74" s="6">
         <v>0.5</v>
       </c>
-      <c r="D74" t="s">
-        <v>66</v>
+      <c r="D74">
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
@@ -1297,8 +1297,8 @@
       <c r="C75" s="6">
         <v>0.5</v>
       </c>
-      <c r="D75" t="s">
-        <v>66</v>
+      <c r="D75">
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:4" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
@@ -1328,11 +1328,26 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010075D40D9C3EDB8943872FF524C6B3FD0A" ma:contentTypeVersion="3" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="c8b69379abfde7286eda3659b10c0c3d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0dd4ebbd-e603-4963-8782-ab9329a1459d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="455ee242f80cd7a09b1a6ea5707d2ed2" ns2:_="">
     <xsd:import namespace="0dd4ebbd-e603-4963-8782-ab9329a1459d"/>
@@ -1470,22 +1485,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{981279ED-D6DF-4F74-A002-827C305FADC6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3CEAD3D1-BC7F-4367-835C-54F9567E9A4E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{536D9EC2-1905-4286-971A-18C563B29D4A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1501,21 +1518,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3CEAD3D1-BC7F-4367-835C-54F9567E9A4E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{981279ED-D6DF-4F74-A002-827C305FADC6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>